<commit_message>
BlackBox Testcase - Quan Ly Tai Lieu
</commit_message>
<xml_diff>
--- a/Docs/SE07_BlackBoxTestCase_v1.0.xlsx
+++ b/Docs/SE07_BlackBoxTestCase_v1.0.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="8190" tabRatio="840" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="8190" tabRatio="840" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -14,13 +14,15 @@
     <sheet name="Check QLKT-CN screen" sheetId="7" r:id="rId5"/>
     <sheet name="Check QLKT-TM screen" sheetId="6" r:id="rId6"/>
     <sheet name="Test Report" sheetId="5" r:id="rId7"/>
+    <sheet name="Check QLTL-DS screen" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Check Login Screen'!$A$8:$H$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Check QLKT-DS screen'!$A$8:$H$21</definedName>
     <definedName name="ACTION">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -210,8 +212,36 @@
 </comments>
 </file>
 
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="F8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="8"/>
+            <rFont val="Times New Roman"/>
+            <family val="1"/>
+          </rPr>
+          <t xml:space="preserve">Pass
+Fail
+Untested
+N/A
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="243">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -979,6 +1009,45 @@
   <si>
     <t>Check Quản lý kỳ thi - 
 Thêm mới Screen</t>
+  </si>
+  <si>
+    <t>Check Quản lý tài liệu - Danh sách  Screen</t>
+  </si>
+  <si>
+    <t>Gui-QLTL_DS-1</t>
+  </si>
+  <si>
+    <t>[Tên tài liệu] Column</t>
+  </si>
+  <si>
+    <t>[Tác giả] Column</t>
+  </si>
+  <si>
+    <t>[Năm xuất bản] Column</t>
+  </si>
+  <si>
+    <t>[Ngày cập nhật] Column</t>
+  </si>
+  <si>
+    <t>Lấy dữ liệu từ cột Tên tài liệu trong bảng Tài liệu</t>
+  </si>
+  <si>
+    <t>Lấy dữ liệu từ cột Tên tác giả trong bảng Tài liệu</t>
+  </si>
+  <si>
+    <t>Lấy dữ liệu từ cột Năm xuất bản trong bản Tài liệu</t>
+  </si>
+  <si>
+    <t>Lấy dữ liệu số thí sinh tham gia trong bản Tài liệu</t>
+  </si>
+  <si>
+    <t>Gui-QLTL_DS-2</t>
+  </si>
+  <si>
+    <t>Gui-QLTL_DS-3</t>
+  </si>
+  <si>
+    <t>Gui-QLTL_DS-4</t>
   </si>
 </sst>
 </file>
@@ -2289,6 +2358,27 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2339,27 +2429,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2749,13 +2818,13 @@
     <row r="2" spans="1:7" s="5" customFormat="1" ht="75.75" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="176" t="s">
+      <c r="C2" s="183" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
+      <c r="D2" s="183"/>
+      <c r="E2" s="183"/>
+      <c r="F2" s="183"/>
+      <c r="G2" s="183"/>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" s="6"/>
@@ -2766,11 +2835,11 @@
       <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="177" t="s">
+      <c r="C4" s="184" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="177"/>
-      <c r="E4" s="177"/>
+      <c r="D4" s="184"/>
+      <c r="E4" s="184"/>
       <c r="F4" s="9" t="s">
         <v>3</v>
       </c>
@@ -2780,36 +2849,36 @@
       <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="177" t="s">
+      <c r="C5" s="184" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="177"/>
-      <c r="E5" s="177"/>
+      <c r="D5" s="184"/>
+      <c r="E5" s="184"/>
       <c r="F5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B6" s="178" t="s">
+      <c r="B6" s="185" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="179" t="str">
+      <c r="C6" s="186" t="str">
         <f>C5&amp;"_"&amp;"XXX"&amp;"_"&amp;"vx.x"</f>
         <v>&lt;Project Code&gt;_XXX_vx.x</v>
       </c>
-      <c r="D6" s="179"/>
-      <c r="E6" s="179"/>
+      <c r="D6" s="186"/>
+      <c r="E6" s="186"/>
       <c r="F6" s="9" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" ht="13.5" customHeight="1">
-      <c r="B7" s="178"/>
-      <c r="C7" s="179"/>
-      <c r="D7" s="179"/>
-      <c r="E7" s="179"/>
+      <c r="B7" s="185"/>
+      <c r="C7" s="186"/>
+      <c r="D7" s="186"/>
+      <c r="E7" s="186"/>
       <c r="F7" s="9" t="s">
         <v>9</v>
       </c>
@@ -2965,39 +3034,39 @@
       <c r="E2" s="42"/>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="182" t="s">
+      <c r="B3" s="189" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="182"/>
-      <c r="D3" s="183" t="str">
+      <c r="C3" s="189"/>
+      <c r="D3" s="190" t="str">
         <f>Cover!C4</f>
         <v>&lt;Project Name&gt;</v>
       </c>
-      <c r="E3" s="183"/>
-      <c r="F3" s="183"/>
+      <c r="E3" s="190"/>
+      <c r="F3" s="190"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="182" t="s">
+      <c r="B4" s="189" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="182"/>
-      <c r="D4" s="183" t="str">
+      <c r="C4" s="189"/>
+      <c r="D4" s="190" t="str">
         <f>Cover!C5</f>
         <v>&lt;Project Code&gt;</v>
       </c>
-      <c r="E4" s="183"/>
-      <c r="F4" s="183"/>
+      <c r="E4" s="190"/>
+      <c r="F4" s="190"/>
     </row>
     <row r="5" spans="2:6" s="43" customFormat="1" ht="84.75" customHeight="1">
-      <c r="B5" s="180" t="s">
+      <c r="B5" s="187" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="180"/>
-      <c r="D5" s="181" t="s">
+      <c r="C5" s="187"/>
+      <c r="D5" s="188" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="181"/>
-      <c r="F5" s="181"/>
+      <c r="E5" s="188"/>
+      <c r="F5" s="188"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="44"/>
@@ -3115,7 +3184,7 @@
       <c r="C15" s="150" t="s">
         <v>226</v>
       </c>
-      <c r="D15" s="194" t="s">
+      <c r="D15" s="176" t="s">
         <v>186</v>
       </c>
       <c r="E15" s="58"/>
@@ -3141,7 +3210,7 @@
       <c r="C17" s="55" t="s">
         <v>228</v>
       </c>
-      <c r="D17" s="194" t="s">
+      <c r="D17" s="176" t="s">
         <v>224</v>
       </c>
       <c r="E17" s="58"/>
@@ -3210,7 +3279,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3243,13 +3312,13 @@
       <c r="A2" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="185" t="s">
+      <c r="B2" s="192" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="185"/>
-      <c r="D2" s="185"/>
-      <c r="E2" s="185"/>
-      <c r="F2" s="185"/>
+      <c r="C2" s="192"/>
+      <c r="D2" s="192"/>
+      <c r="E2" s="192"/>
+      <c r="F2" s="192"/>
       <c r="G2" s="72"/>
       <c r="H2" s="43"/>
       <c r="I2" s="69"/>
@@ -3261,13 +3330,13 @@
       <c r="A3" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="185" t="s">
+      <c r="B3" s="192" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="185"/>
-      <c r="D3" s="185"/>
-      <c r="E3" s="185"/>
-      <c r="F3" s="185"/>
+      <c r="C3" s="192"/>
+      <c r="D3" s="192"/>
+      <c r="E3" s="192"/>
+      <c r="F3" s="192"/>
       <c r="G3" s="72"/>
       <c r="H3" s="43"/>
       <c r="I3" s="69"/>
@@ -3279,11 +3348,11 @@
       <c r="A4" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="186"/>
-      <c r="C4" s="186"/>
-      <c r="D4" s="186"/>
-      <c r="E4" s="186"/>
-      <c r="F4" s="186"/>
+      <c r="B4" s="193"/>
+      <c r="C4" s="193"/>
+      <c r="D4" s="193"/>
+      <c r="E4" s="193"/>
+      <c r="F4" s="193"/>
       <c r="G4" s="72"/>
       <c r="H4" s="43"/>
       <c r="I4" s="69"/>
@@ -3302,10 +3371,10 @@
       <c r="D5" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="187" t="s">
+      <c r="E5" s="194" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="187"/>
+      <c r="F5" s="194"/>
       <c r="G5" s="78"/>
       <c r="H5" s="78"/>
       <c r="I5" s="79"/>
@@ -3330,11 +3399,11 @@
         <f>COUNTIF(F$10:F$1002,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="184">
+      <c r="E6" s="191">
         <f>COUNTA(A10:A1002)</f>
         <v>11</v>
       </c>
-      <c r="F6" s="184"/>
+      <c r="F6" s="191"/>
       <c r="G6" s="78"/>
       <c r="H6" s="78"/>
       <c r="I6" s="79"/>
@@ -3668,9 +3737,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3703,13 +3772,13 @@
       <c r="A2" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="185" t="s">
+      <c r="B2" s="192" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="185"/>
-      <c r="D2" s="185"/>
-      <c r="E2" s="185"/>
-      <c r="F2" s="185"/>
+      <c r="C2" s="192"/>
+      <c r="D2" s="192"/>
+      <c r="E2" s="192"/>
+      <c r="F2" s="192"/>
       <c r="G2" s="72"/>
       <c r="H2" s="43"/>
       <c r="I2" s="69"/>
@@ -3721,13 +3790,13 @@
       <c r="A3" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="185" t="s">
+      <c r="B3" s="192" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="185"/>
-      <c r="D3" s="185"/>
-      <c r="E3" s="185"/>
-      <c r="F3" s="185"/>
+      <c r="C3" s="192"/>
+      <c r="D3" s="192"/>
+      <c r="E3" s="192"/>
+      <c r="F3" s="192"/>
       <c r="G3" s="72"/>
       <c r="H3" s="43"/>
       <c r="I3" s="69"/>
@@ -3739,11 +3808,11 @@
       <c r="A4" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="186"/>
-      <c r="C4" s="186"/>
-      <c r="D4" s="186"/>
-      <c r="E4" s="186"/>
-      <c r="F4" s="186"/>
+      <c r="B4" s="193"/>
+      <c r="C4" s="193"/>
+      <c r="D4" s="193"/>
+      <c r="E4" s="193"/>
+      <c r="F4" s="193"/>
       <c r="G4" s="72"/>
       <c r="H4" s="43"/>
       <c r="I4" s="69"/>
@@ -3762,10 +3831,10 @@
       <c r="D5" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="187" t="s">
+      <c r="E5" s="194" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="187"/>
+      <c r="F5" s="194"/>
       <c r="G5" s="78"/>
       <c r="H5" s="78"/>
       <c r="I5" s="79"/>
@@ -3790,11 +3859,11 @@
         <f>COUNTIF(F$10:F$1004,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="184">
+      <c r="E6" s="191">
         <f>COUNTA(A10:A1004)</f>
         <v>6</v>
       </c>
-      <c r="F6" s="184"/>
+      <c r="F6" s="191"/>
       <c r="G6" s="78"/>
       <c r="H6" s="78"/>
       <c r="I6" s="79"/>
@@ -3870,10 +3939,10 @@
       <c r="I10" s="95"/>
     </row>
     <row r="11" spans="1:10" ht="25.5">
-      <c r="A11" s="188" t="s">
+      <c r="A11" s="195" t="s">
         <v>103</v>
       </c>
-      <c r="B11" s="188" t="s">
+      <c r="B11" s="195" t="s">
         <v>104</v>
       </c>
       <c r="C11" s="159"/>
@@ -3889,8 +3958,8 @@
       <c r="I11" s="95"/>
     </row>
     <row r="12" spans="1:10" ht="25.5">
-      <c r="A12" s="189"/>
-      <c r="B12" s="189"/>
+      <c r="A12" s="196"/>
+      <c r="B12" s="196"/>
       <c r="C12" s="159" t="s">
         <v>106</v>
       </c>
@@ -3904,8 +3973,8 @@
       <c r="I12" s="95"/>
     </row>
     <row r="13" spans="1:10" ht="25.5">
-      <c r="A13" s="189"/>
-      <c r="B13" s="189"/>
+      <c r="A13" s="196"/>
+      <c r="B13" s="196"/>
       <c r="C13" s="159" t="s">
         <v>107</v>
       </c>
@@ -3919,8 +3988,8 @@
       <c r="I13" s="95"/>
     </row>
     <row r="14" spans="1:10" ht="25.5">
-      <c r="A14" s="189"/>
-      <c r="B14" s="189"/>
+      <c r="A14" s="196"/>
+      <c r="B14" s="196"/>
       <c r="C14" s="160" t="s">
         <v>108</v>
       </c>
@@ -3934,8 +4003,8 @@
       <c r="I14" s="95"/>
     </row>
     <row r="15" spans="1:10" ht="25.5">
-      <c r="A15" s="189"/>
-      <c r="B15" s="189"/>
+      <c r="A15" s="196"/>
+      <c r="B15" s="196"/>
       <c r="C15" s="160" t="s">
         <v>109</v>
       </c>
@@ -3949,8 +4018,8 @@
       <c r="I15" s="95"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="190"/>
-      <c r="B16" s="190"/>
+      <c r="A16" s="197"/>
+      <c r="B16" s="197"/>
       <c r="C16" s="160" t="s">
         <v>110</v>
       </c>
@@ -4131,13 +4200,13 @@
       <c r="A2" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="185" t="s">
+      <c r="B2" s="192" t="s">
         <v>187</v>
       </c>
-      <c r="C2" s="185"/>
-      <c r="D2" s="185"/>
-      <c r="E2" s="185"/>
-      <c r="F2" s="185"/>
+      <c r="C2" s="192"/>
+      <c r="D2" s="192"/>
+      <c r="E2" s="192"/>
+      <c r="F2" s="192"/>
       <c r="G2" s="72"/>
       <c r="H2" s="43"/>
       <c r="I2" s="69"/>
@@ -4149,13 +4218,13 @@
       <c r="A3" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="185" t="s">
+      <c r="B3" s="192" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="185"/>
-      <c r="D3" s="185"/>
-      <c r="E3" s="185"/>
-      <c r="F3" s="185"/>
+      <c r="C3" s="192"/>
+      <c r="D3" s="192"/>
+      <c r="E3" s="192"/>
+      <c r="F3" s="192"/>
       <c r="G3" s="72"/>
       <c r="H3" s="43"/>
       <c r="I3" s="69"/>
@@ -4167,11 +4236,11 @@
       <c r="A4" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="186"/>
-      <c r="C4" s="186"/>
-      <c r="D4" s="186"/>
-      <c r="E4" s="186"/>
-      <c r="F4" s="186"/>
+      <c r="B4" s="193"/>
+      <c r="C4" s="193"/>
+      <c r="D4" s="193"/>
+      <c r="E4" s="193"/>
+      <c r="F4" s="193"/>
       <c r="G4" s="72"/>
       <c r="H4" s="43"/>
       <c r="I4" s="69"/>
@@ -4190,10 +4259,10 @@
       <c r="D5" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="187" t="s">
+      <c r="E5" s="194" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="187"/>
+      <c r="F5" s="194"/>
       <c r="G5" s="78"/>
       <c r="H5" s="78"/>
       <c r="I5" s="79"/>
@@ -4218,11 +4287,11 @@
         <f>COUNTIF(F$10:F$1008,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="184">
+      <c r="E6" s="191">
         <f>COUNTA(A10:A1009)</f>
         <v>14</v>
       </c>
-      <c r="F6" s="184"/>
+      <c r="F6" s="191"/>
       <c r="G6" s="78"/>
       <c r="H6" s="78"/>
       <c r="I6" s="79"/>
@@ -4665,13 +4734,13 @@
       <c r="A2" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="185" t="s">
+      <c r="B2" s="192" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="185"/>
-      <c r="D2" s="185"/>
-      <c r="E2" s="185"/>
-      <c r="F2" s="185"/>
+      <c r="C2" s="192"/>
+      <c r="D2" s="192"/>
+      <c r="E2" s="192"/>
+      <c r="F2" s="192"/>
       <c r="G2" s="72"/>
       <c r="H2" s="43"/>
       <c r="I2" s="69"/>
@@ -4683,13 +4752,13 @@
       <c r="A3" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="185" t="s">
+      <c r="B3" s="192" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="185"/>
-      <c r="D3" s="185"/>
-      <c r="E3" s="185"/>
-      <c r="F3" s="185"/>
+      <c r="C3" s="192"/>
+      <c r="D3" s="192"/>
+      <c r="E3" s="192"/>
+      <c r="F3" s="192"/>
       <c r="G3" s="72"/>
       <c r="H3" s="43"/>
       <c r="I3" s="69"/>
@@ -4701,11 +4770,11 @@
       <c r="A4" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="186"/>
-      <c r="C4" s="186"/>
-      <c r="D4" s="186"/>
-      <c r="E4" s="186"/>
-      <c r="F4" s="186"/>
+      <c r="B4" s="193"/>
+      <c r="C4" s="193"/>
+      <c r="D4" s="193"/>
+      <c r="E4" s="193"/>
+      <c r="F4" s="193"/>
       <c r="G4" s="72"/>
       <c r="H4" s="43"/>
       <c r="I4" s="69"/>
@@ -4724,10 +4793,10 @@
       <c r="D5" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="187" t="s">
+      <c r="E5" s="194" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="187"/>
+      <c r="F5" s="194"/>
       <c r="G5" s="78"/>
       <c r="H5" s="78"/>
       <c r="I5" s="79"/>
@@ -4752,11 +4821,11 @@
         <f>COUNTIF(F$10:F$1011,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="184">
+      <c r="E6" s="191">
         <f>COUNTA(A10:A1012)</f>
         <v>17</v>
       </c>
-      <c r="F6" s="184"/>
+      <c r="F6" s="191"/>
       <c r="G6" s="78"/>
       <c r="H6" s="78"/>
       <c r="I6" s="79"/>
@@ -5218,7 +5287,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5232,15 +5301,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.5" customHeight="1">
-      <c r="B1" s="193" t="s">
+      <c r="B1" s="200" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="193"/>
-      <c r="D1" s="193"/>
-      <c r="E1" s="193"/>
-      <c r="F1" s="193"/>
-      <c r="G1" s="193"/>
-      <c r="H1" s="193"/>
+      <c r="C1" s="200"/>
+      <c r="D1" s="200"/>
+      <c r="E1" s="200"/>
+      <c r="F1" s="200"/>
+      <c r="G1" s="200"/>
+      <c r="H1" s="200"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1">
       <c r="A2" s="105"/>
@@ -5256,14 +5325,14 @@
       <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="183" t="s">
+      <c r="C3" s="190" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="183"/>
-      <c r="E3" s="191" t="s">
+      <c r="D3" s="190"/>
+      <c r="E3" s="198" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="191"/>
+      <c r="F3" s="198"/>
       <c r="G3" s="108"/>
       <c r="H3" s="109"/>
     </row>
@@ -5271,14 +5340,14 @@
       <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="183" t="s">
+      <c r="C4" s="190" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="183"/>
-      <c r="E4" s="191" t="s">
+      <c r="D4" s="190"/>
+      <c r="E4" s="198" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="191"/>
+      <c r="F4" s="198"/>
       <c r="G4" s="108"/>
       <c r="H4" s="109"/>
     </row>
@@ -5286,15 +5355,15 @@
       <c r="B5" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="183" t="str">
+      <c r="C5" s="190" t="str">
         <f>C4&amp;"_"&amp;"Test Report"&amp;"_"&amp;"vx.x"</f>
         <v>&lt;Project Code&gt;_Test Report_vx.x</v>
       </c>
-      <c r="D5" s="183"/>
-      <c r="E5" s="191" t="s">
+      <c r="D5" s="190"/>
+      <c r="E5" s="198" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="191"/>
+      <c r="F5" s="198"/>
       <c r="G5" s="108"/>
       <c r="H5" s="111" t="s">
         <v>44</v>
@@ -5305,14 +5374,14 @@
       <c r="B6" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="192" t="s">
+      <c r="C6" s="199" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="192"/>
-      <c r="E6" s="192"/>
-      <c r="F6" s="192"/>
-      <c r="G6" s="192"/>
-      <c r="H6" s="192"/>
+      <c r="D6" s="199"/>
+      <c r="E6" s="199"/>
+      <c r="F6" s="199"/>
+      <c r="G6" s="199"/>
+      <c r="H6" s="199"/>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1">
       <c r="A7" s="105"/>
@@ -5432,7 +5501,7 @@
       <c r="B13" s="122">
         <v>3</v>
       </c>
-      <c r="C13" s="195" t="s">
+      <c r="C13" s="177" t="s">
         <v>229</v>
       </c>
       <c r="D13" s="124">
@@ -5447,19 +5516,19 @@
     </row>
     <row r="14" spans="1:8" ht="25.5">
       <c r="A14" s="121"/>
-      <c r="B14" s="196">
+      <c r="B14" s="178">
         <v>4</v>
       </c>
-      <c r="C14" s="197" t="s">
+      <c r="C14" s="179" t="s">
         <v>187</v>
       </c>
-      <c r="D14" s="198">
+      <c r="D14" s="180">
         <v>14</v>
       </c>
-      <c r="E14" s="198"/>
-      <c r="F14" s="198"/>
-      <c r="G14" s="199"/>
-      <c r="H14" s="200">
+      <c r="E14" s="180"/>
+      <c r="F14" s="180"/>
+      <c r="G14" s="181"/>
+      <c r="H14" s="182">
         <v>14</v>
       </c>
     </row>
@@ -5556,4 +5625,436 @@
     <oddFooter>&amp;L&amp;"Tahoma,Regular"&amp;8 02ae-BM/PM/HDCV/FSOFT v2/0&amp;C&amp;"tahoma,Regular"&amp;8Internal use&amp;R&amp;"Tahoma,Regular"&amp;8&amp;P/&amp;N</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="11.5" style="8" customWidth="1"/>
+    <col min="2" max="2" width="19.125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="25.625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="30.125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="16.875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="7.125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="9" style="63"/>
+    <col min="8" max="8" width="17.625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="8.25" style="64" customWidth="1"/>
+    <col min="10" max="10" width="0" style="8" hidden="1" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="70" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A1" s="65"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="69"/>
+    </row>
+    <row r="2" spans="1:10" s="70" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="71" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="192" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" s="192"/>
+      <c r="D2" s="192"/>
+      <c r="E2" s="192"/>
+      <c r="F2" s="192"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="70" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="70" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A3" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="192" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="192"/>
+      <c r="D3" s="192"/>
+      <c r="E3" s="192"/>
+      <c r="F3" s="192"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="70" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="70" customFormat="1" ht="18" customHeight="1">
+      <c r="A4" s="71" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="193"/>
+      <c r="C4" s="193"/>
+      <c r="D4" s="193"/>
+      <c r="E4" s="193"/>
+      <c r="F4" s="193"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="74"/>
+    </row>
+    <row r="5" spans="1:10" s="70" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A5" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="76" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="77" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="194" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="194"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="70" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="70" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A6" s="101">
+        <v>2</v>
+      </c>
+      <c r="B6" s="81">
+        <f>COUNTIF(F10:F1004,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="81">
+        <f>E6-D6-B6-A6</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="82">
+        <f>COUNTIF(F$10:F$1004,"N/A")</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="191">
+        <v>2</v>
+      </c>
+      <c r="F6" s="191"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="70" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="70" customFormat="1" ht="15" customHeight="1">
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="79"/>
+    </row>
+    <row r="8" spans="1:10" s="70" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A8" s="84" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="84" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="84" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="84" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="85" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="85" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="85" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="84" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="86"/>
+    </row>
+    <row r="9" spans="1:10" s="70" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A9" s="87"/>
+      <c r="B9" s="87" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="89"/>
+      <c r="I9" s="90"/>
+    </row>
+    <row r="10" spans="1:10" s="96" customFormat="1" ht="120.95" customHeight="1">
+      <c r="A10" s="141" t="s">
+        <v>231</v>
+      </c>
+      <c r="B10" s="157" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="153"/>
+      <c r="D10" s="151" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="154"/>
+      <c r="F10" s="91" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="91"/>
+      <c r="H10" s="102"/>
+      <c r="I10" s="95"/>
+    </row>
+    <row r="11" spans="1:10" ht="25.5">
+      <c r="A11" s="195" t="s">
+        <v>240</v>
+      </c>
+      <c r="B11" s="195" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="159"/>
+      <c r="D11" s="147" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="148"/>
+      <c r="F11" s="152" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="91"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="95"/>
+    </row>
+    <row r="12" spans="1:10" ht="25.5">
+      <c r="A12" s="196"/>
+      <c r="B12" s="196"/>
+      <c r="C12" s="159" t="s">
+        <v>232</v>
+      </c>
+      <c r="D12" s="147" t="s">
+        <v>236</v>
+      </c>
+      <c r="E12" s="148"/>
+      <c r="F12" s="152"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="102"/>
+      <c r="I12" s="95"/>
+    </row>
+    <row r="13" spans="1:10" ht="25.5">
+      <c r="A13" s="196"/>
+      <c r="B13" s="196"/>
+      <c r="C13" s="159" t="s">
+        <v>233</v>
+      </c>
+      <c r="D13" s="147" t="s">
+        <v>237</v>
+      </c>
+      <c r="E13" s="148"/>
+      <c r="F13" s="152"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="102"/>
+      <c r="I13" s="95"/>
+    </row>
+    <row r="14" spans="1:10" ht="25.5">
+      <c r="A14" s="196"/>
+      <c r="B14" s="196"/>
+      <c r="C14" s="160" t="s">
+        <v>234</v>
+      </c>
+      <c r="D14" s="155" t="s">
+        <v>238</v>
+      </c>
+      <c r="E14" s="158"/>
+      <c r="F14" s="152"/>
+      <c r="G14" s="91"/>
+      <c r="H14" s="102"/>
+      <c r="I14" s="95"/>
+    </row>
+    <row r="15" spans="1:10" ht="25.5">
+      <c r="A15" s="196"/>
+      <c r="B15" s="196"/>
+      <c r="C15" s="160" t="s">
+        <v>235</v>
+      </c>
+      <c r="D15" s="155" t="s">
+        <v>239</v>
+      </c>
+      <c r="E15" s="158"/>
+      <c r="F15" s="152"/>
+      <c r="G15" s="91"/>
+      <c r="H15" s="102"/>
+      <c r="I15" s="95"/>
+    </row>
+    <row r="16" spans="1:10" ht="25.5">
+      <c r="A16" s="197"/>
+      <c r="B16" s="197"/>
+      <c r="C16" s="160" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="155" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="158"/>
+      <c r="F16" s="152"/>
+      <c r="G16" s="91"/>
+      <c r="H16" s="102"/>
+      <c r="I16" s="95"/>
+    </row>
+    <row r="17" spans="1:11" ht="25.5">
+      <c r="A17" s="162" t="s">
+        <v>241</v>
+      </c>
+      <c r="B17" s="163" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="164"/>
+      <c r="D17" s="156" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="165"/>
+      <c r="F17" s="166" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="141"/>
+      <c r="H17" s="167"/>
+      <c r="I17" s="95"/>
+    </row>
+    <row r="18" spans="1:11" ht="25.5">
+      <c r="A18" s="142" t="s">
+        <v>242</v>
+      </c>
+      <c r="B18" s="142" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="142"/>
+      <c r="D18" s="147" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="148"/>
+      <c r="F18" s="142" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="142"/>
+      <c r="H18" s="169"/>
+      <c r="I18" s="95"/>
+    </row>
+    <row r="19" spans="1:11" s="70" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A19" s="146"/>
+      <c r="B19" s="146" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="140"/>
+      <c r="D19" s="140"/>
+      <c r="E19" s="140"/>
+      <c r="F19" s="140"/>
+      <c r="G19" s="140"/>
+      <c r="H19" s="168"/>
+      <c r="I19" s="90"/>
+    </row>
+    <row r="20" spans="1:11" ht="178.5">
+      <c r="A20" s="91" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="91" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" s="149" t="s">
+        <v>127</v>
+      </c>
+      <c r="D20" s="149" t="s">
+        <v>124</v>
+      </c>
+      <c r="E20" s="91"/>
+      <c r="F20" s="91" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="91"/>
+      <c r="H20" s="102"/>
+      <c r="I20" s="95"/>
+    </row>
+    <row r="21" spans="1:11" ht="153">
+      <c r="A21" s="91" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="91" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="149" t="s">
+        <v>127</v>
+      </c>
+      <c r="D21" s="149" t="s">
+        <v>128</v>
+      </c>
+      <c r="E21" s="91"/>
+      <c r="F21" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="98"/>
+      <c r="H21" s="99"/>
+      <c r="I21" s="100"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="F22" s="103"/>
+      <c r="I22" s="90"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="70"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="F23" s="104"/>
+      <c r="I23" s="95"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="B11:B16"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F3 F7:F150">
+      <formula1>$J$2:$J$6</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Update BlackBox Testcase"
This reverts commit 88db919bf42ae4bd1e75c881c37f6bbc1cd287d5.
</commit_message>
<xml_diff>
--- a/Docs/SE07_BlackBoxTestCase_v1.0.xlsx
+++ b/Docs/SE07_BlackBoxTestCase_v1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="8190" tabRatio="840" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="8190" tabRatio="840" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -241,7 +241,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="243">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -1035,6 +1035,12 @@
     <t>Lấy dữ liệu từ cột Tên tác giả trong bảng Tài liệu</t>
   </si>
   <si>
+    <t>Lấy dữ liệu từ cột Năm xuất bản trong bản Tài liệu</t>
+  </si>
+  <si>
+    <t>Lấy dữ liệu số thí sinh tham gia trong bản Tài liệu</t>
+  </si>
+  <si>
     <t>Gui-QLTL_DS-2</t>
   </si>
   <si>
@@ -1042,26 +1048,6 @@
   </si>
   <si>
     <t>Gui-QLTL_DS-4</t>
-  </si>
-  <si>
-    <t>Lấy dữ liệu từ cột Năm xuất bản trong bảng Tài liệu</t>
-  </si>
-  <si>
-    <t>Lấy dữ liệu số thí sinh tham gia trong bảng Tài liệu</t>
-  </si>
-  <si>
-    <t>- Tại màn hình quản lý tài liệu - danh sách
-1. Click vào linkbutton xóa
-2. Click vào xác nhận xóa</t>
-  </si>
-  <si>
-    <t>Check GUI-Quản lí tài liệu - Danh sách Screen</t>
-  </si>
-  <si>
-    <t>Check QLTL-DS screen</t>
-  </si>
-  <si>
-    <t>Check Function xoá</t>
   </si>
 </sst>
 </file>
@@ -3020,16 +3006,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="1.375" style="8" customWidth="1"/>
     <col min="2" max="2" width="11.75" style="37" customWidth="1"/>
-    <col min="3" max="3" width="34.25" style="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.125" style="38" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5" style="38" customWidth="1"/>
+    <col min="4" max="4" width="17.125" style="38" customWidth="1"/>
     <col min="5" max="5" width="28.125" style="38" customWidth="1"/>
     <col min="6" max="6" width="30.625" style="38" customWidth="1"/>
     <col min="7" max="16384" width="9" style="8"/>
@@ -3230,29 +3216,17 @@
       <c r="E17" s="58"/>
       <c r="F17" s="57"/>
     </row>
-    <row r="18" spans="2:6" ht="13.5">
-      <c r="B18" s="54">
-        <v>10</v>
-      </c>
-      <c r="C18" s="55" t="s">
-        <v>244</v>
-      </c>
-      <c r="D18" s="175" t="s">
-        <v>245</v>
-      </c>
+    <row r="18" spans="2:6">
+      <c r="B18" s="54"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="58"/>
       <c r="E18" s="58"/>
       <c r="F18" s="57"/>
     </row>
-    <row r="19" spans="2:6" ht="13.5">
-      <c r="B19" s="54">
-        <v>11</v>
-      </c>
-      <c r="C19" s="55" t="s">
-        <v>246</v>
-      </c>
-      <c r="D19" s="175" t="s">
-        <v>245</v>
-      </c>
+    <row r="19" spans="2:6">
+      <c r="B19" s="54"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="58"/>
       <c r="E19" s="58"/>
       <c r="F19" s="57"/>
     </row>
@@ -3290,8 +3264,6 @@
     <hyperlink ref="D15" location="'Check QLKT-TM screen'!A1" display="Check QLKT-TM screen"/>
     <hyperlink ref="D16" location="'Check QLKT-CN screen'!A1" display="Check QLKT-CN screen"/>
     <hyperlink ref="D17" location="'Check QLKT-CN screen'!A1" display="Check QLKT-CN screen"/>
-    <hyperlink ref="D18" location="'Check QLTL-DS screen'!A1" display="'Check QLTL-DS screen'!A1"/>
-    <hyperlink ref="D19" location="'Check QLTL-DS screen'!A1" display="'Check QLTL-DS screen'!A1"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777783" bottom="1.1506944444444445" header="0.51180555555555562" footer="0.98402777777777783"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5659,7 +5631,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -5763,7 +5737,7 @@
     </row>
     <row r="6" spans="1:10" s="70" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="101">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B6" s="81">
         <f>COUNTIF(F10:F1004,"Fail")</f>
@@ -5778,7 +5752,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="191">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F6" s="191"/>
       <c r="G6" s="78"/>
@@ -5857,7 +5831,7 @@
     </row>
     <row r="11" spans="1:10" ht="25.5">
       <c r="A11" s="195" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B11" s="195" t="s">
         <v>104</v>
@@ -5911,7 +5885,7 @@
         <v>234</v>
       </c>
       <c r="D14" s="155" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E14" s="158"/>
       <c r="F14" s="152"/>
@@ -5926,7 +5900,7 @@
         <v>235</v>
       </c>
       <c r="D15" s="155" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E15" s="158"/>
       <c r="F15" s="152"/>
@@ -5934,7 +5908,7 @@
       <c r="H15" s="102"/>
       <c r="I15" s="95"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" ht="25.5">
       <c r="A16" s="197"/>
       <c r="B16" s="197"/>
       <c r="C16" s="160" t="s">
@@ -5951,7 +5925,7 @@
     </row>
     <row r="17" spans="1:11" ht="25.5">
       <c r="A17" s="162" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B17" s="163" t="s">
         <v>117</v>
@@ -5970,7 +5944,7 @@
     </row>
     <row r="18" spans="1:11" ht="25.5">
       <c r="A18" s="142" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B18" s="142" t="s">
         <v>119</v>
@@ -6000,7 +5974,7 @@
       <c r="H19" s="168"/>
       <c r="I19" s="90"/>
     </row>
-    <row r="20" spans="1:11" ht="51">
+    <row r="20" spans="1:11" ht="178.5">
       <c r="A20" s="91" t="s">
         <v>122</v>
       </c>
@@ -6008,7 +5982,7 @@
         <v>123</v>
       </c>
       <c r="C20" s="149" t="s">
-        <v>243</v>
+        <v>127</v>
       </c>
       <c r="D20" s="149" t="s">
         <v>124</v>
@@ -6021,7 +5995,7 @@
       <c r="H20" s="102"/>
       <c r="I20" s="95"/>
     </row>
-    <row r="21" spans="1:11" ht="51">
+    <row r="21" spans="1:11" ht="153">
       <c r="A21" s="91" t="s">
         <v>125</v>
       </c>
@@ -6029,7 +6003,7 @@
         <v>126</v>
       </c>
       <c r="C21" s="149" t="s">
-        <v>243</v>
+        <v>127</v>
       </c>
       <c r="D21" s="149" t="s">
         <v>128</v>
@@ -6054,13 +6028,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A11:A16"/>
-    <mergeCell ref="B11:B16"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="B11:B16"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F3 F7:F150">

</xml_diff>

<commit_message>
Update BlackBox TestCase - QLTL
</commit_message>
<xml_diff>
--- a/Docs/SE07_BlackBoxTestCase_v1.0.xlsx
+++ b/Docs/SE07_BlackBoxTestCase_v1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="8190" tabRatio="840" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="8190" tabRatio="840" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="Check QLKT-TM screen" sheetId="6" r:id="rId6"/>
     <sheet name="Test Report" sheetId="5" r:id="rId7"/>
     <sheet name="Check QLTL-DS screen" sheetId="8" r:id="rId8"/>
-    <sheet name="Sheet2" sheetId="9" r:id="rId9"/>
+    <sheet name="Check QLTL-CN screen" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Check Login Screen'!$A$8:$H$21</definedName>
@@ -240,8 +240,36 @@
 </comments>
 </file>
 
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="F8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="8"/>
+            <rFont val="Times New Roman"/>
+            <family val="1"/>
+          </rPr>
+          <t xml:space="preserve">Pass
+Fail
+Untested
+N/A
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="289">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -1048,6 +1076,173 @@
   </si>
   <si>
     <t>Gui-QLTL_DS-4</t>
+  </si>
+  <si>
+    <t>- Tại màn hình quản lý tài liệu - danh sách
+1. Click vào linkbutton xóa
+2. Click vào xác nhận xóa</t>
+  </si>
+  <si>
+    <t>Check GUI-Quản lí tài liệu - Danh sách</t>
+  </si>
+  <si>
+    <t>Check QLTL-DS screen'</t>
+  </si>
+  <si>
+    <t>Check Function xoá</t>
+  </si>
+  <si>
+    <t>Check Quản lí tài liệu - Danh sách Screen</t>
+  </si>
+  <si>
+    <t>Check Quản lý tài liệu - Sửa Screen</t>
+  </si>
+  <si>
+    <t>Gui-QLTL_CN-1</t>
+  </si>
+  <si>
+    <t>[Tên tài liệu] Textbox</t>
+  </si>
+  <si>
+    <t>Gui-QLTL_CN-2</t>
+  </si>
+  <si>
+    <t>Gui-QLTL_CN-3</t>
+  </si>
+  <si>
+    <t>Gui-QLTL_CN-4</t>
+  </si>
+  <si>
+    <t>Gui-QLTL_CN-5</t>
+  </si>
+  <si>
+    <t>[Tên tác giả] Textbox</t>
+  </si>
+  <si>
+    <t>[Năm xuất bản] Textbox</t>
+  </si>
+  <si>
+    <t>Check Gui - Quản lý tài liệu_Danh sách Screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Tại màn hình quản lý tài liệu - danh sách
+1. Click linkbutton Cập nhật
+</t>
+  </si>
+  <si>
+    <t>- Tại màn hình quản lý tài liệu - Cập nhật
+1. Nhập vào toàn bộ những thông tin cần thiết
+2. Click button [Submit]</t>
+  </si>
+  <si>
+    <t>- Tài liệu mới được cập nhật vào DB
+- Đóng cửa sổ Cập nhật
+- Quay lại trang danh sách
+- Làm mới danh sách tài liệu</t>
+  </si>
+  <si>
+    <t>Cập nhật tài khi không nhập trường tên tài liệu hoặc tên tài liệu là các khoảng trắng</t>
+  </si>
+  <si>
+    <t>- Hiển thị thong báo: "tên tài liệu là bắt buộc"</t>
+  </si>
+  <si>
+    <t>Cập nhật tài liệu khi không nhập trường tên tác giả hoặc tên tác giả là những khoảng trắng</t>
+  </si>
+  <si>
+    <t>- Tại màn hình quản lý tài liệu - Cập nhật
+1. Nhập vào toàn bộ những thông tin cần thiết trừ tên tài liệu
+2. Click button [Submit]</t>
+  </si>
+  <si>
+    <t>- Tại màn hình quản lý tài liệu - Cập nhật
+1. Nhập vào toàn bộ những thông tin cần thiết ngoại trừ tên tác giả
+2. Click button [Submit]</t>
+  </si>
+  <si>
+    <t>Cập nhật kỳ thi khi không nhập trường năm xuất bản hoặc năm xuất bản là những khoảng trắng</t>
+  </si>
+  <si>
+    <t>- Tại màn hình quản lý tài liệu - Cập nhật
+1. Nhập vào toàn bộ những thông tin cần thiết ngoại trừ năm xuất bản
+2. Click button [Submit]</t>
+  </si>
+  <si>
+    <t>- Hiển thị thông báo: "tên tác giả là bắt buộc"</t>
+  </si>
+  <si>
+    <t>- Hiển thị thông báo "năm xuất bản là bắt buộc"</t>
+  </si>
+  <si>
+    <t>- Tại màn hình quản lý tài liệu - Cập nhật
+1. Nhập vào"$$$%" vào các textbox
+2. Click button [Submit]</t>
+  </si>
+  <si>
+    <t>Cập nhật tài liệu khi nhập các trường với ký tự đặc biệt</t>
+  </si>
+  <si>
+    <t>Cập nhật tài liệu khi nhập trường tên tài liệu không phải là kí tự</t>
+  </si>
+  <si>
+    <t>- Hiển thị thông báo " Tên tài liệu không được là số"</t>
+  </si>
+  <si>
+    <t>Cập nhật tài liệu với các trường dữ liệu được nhập với độ dài lớn nhất</t>
+  </si>
+  <si>
+    <t>- Tại màn hình quản lý tài liệu - Cập nhật
+1. Nhập vào toàn bộ những thông tin cần thiết với độ dài lớn nhất
+2. Click button [Submit]</t>
+  </si>
+  <si>
+    <t>- Tài liệu mới được thêm vào DB
+- Đóng cửa sổ Cập nhật
+- Quay lại trang danh sách
+- Làm mới danh sách tài liệu</t>
+  </si>
+  <si>
+    <t>- Tại màn hình quản lý tài liệu - Cập nhật
+1. Click vào linkbutton [Thoát]</t>
+  </si>
+  <si>
+    <t>Quay lại màn hình Quản lý tài liệu - danh sách</t>
+  </si>
+  <si>
+    <t>Check Quản lí tài liệu - Sửa Screen</t>
+  </si>
+  <si>
+    <t>- Tại màn hình quản lý tài liệu - Cập nhật
+1. Nhập vào "123" vào trường tên tài liệu
+2. Click button [Submit]</t>
+  </si>
+  <si>
+    <t>Cập nhật tài liệu khi nhập trường Tên tác giả không phải là kí tự</t>
+  </si>
+  <si>
+    <t>- Tại màn hình quản lý tài liệu - Cập nhật
+1. Nhập vào "123" vào trường tên tác giả
+2. Click button [Submit]</t>
+  </si>
+  <si>
+    <t>- Hiển thị thông báo " Tên tác giả không được là số"</t>
+  </si>
+  <si>
+    <t>Cập nhật tài liệu khi nhập trường Năm xuất bản không phải là ngày/tháng/năm</t>
+  </si>
+  <si>
+    <t>- Tại màn hình quản lý tài liệu - Cập nhật
+1. Nhập vào "123abc" vào trường Năm xuất bản
+2. Click button [Submit]</t>
+  </si>
+  <si>
+    <t>- Hiển thị thông báo " Năm xuất bản không đúng định dạng"</t>
+  </si>
+  <si>
+    <t>FUNC-CN-11</t>
+  </si>
+  <si>
+    <t>FUNC-CN-10</t>
   </si>
 </sst>
 </file>
@@ -1882,7 +2077,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="201">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2378,6 +2573,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="39" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2818,13 +3016,13 @@
     <row r="2" spans="1:7" s="5" customFormat="1" ht="75.75" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="183" t="s">
+      <c r="C2" s="184" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="183"/>
-      <c r="E2" s="183"/>
-      <c r="F2" s="183"/>
-      <c r="G2" s="183"/>
+      <c r="D2" s="184"/>
+      <c r="E2" s="184"/>
+      <c r="F2" s="184"/>
+      <c r="G2" s="184"/>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" s="6"/>
@@ -2835,11 +3033,11 @@
       <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="184" t="s">
+      <c r="C4" s="185" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="184"/>
-      <c r="E4" s="184"/>
+      <c r="D4" s="185"/>
+      <c r="E4" s="185"/>
       <c r="F4" s="9" t="s">
         <v>3</v>
       </c>
@@ -2849,36 +3047,36 @@
       <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="184" t="s">
+      <c r="C5" s="185" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="184"/>
-      <c r="E5" s="184"/>
+      <c r="D5" s="185"/>
+      <c r="E5" s="185"/>
       <c r="F5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="10"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B6" s="185" t="s">
+      <c r="B6" s="186" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="186" t="str">
+      <c r="C6" s="187" t="str">
         <f>C5&amp;"_"&amp;"XXX"&amp;"_"&amp;"vx.x"</f>
         <v>&lt;Project Code&gt;_XXX_vx.x</v>
       </c>
-      <c r="D6" s="186"/>
-      <c r="E6" s="186"/>
+      <c r="D6" s="187"/>
+      <c r="E6" s="187"/>
       <c r="F6" s="9" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="1:7" ht="13.5" customHeight="1">
-      <c r="B7" s="185"/>
-      <c r="C7" s="186"/>
-      <c r="D7" s="186"/>
-      <c r="E7" s="186"/>
+      <c r="B7" s="186"/>
+      <c r="C7" s="187"/>
+      <c r="D7" s="187"/>
+      <c r="E7" s="187"/>
       <c r="F7" s="9" t="s">
         <v>9</v>
       </c>
@@ -3006,16 +3204,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="1.375" style="8" customWidth="1"/>
     <col min="2" max="2" width="11.75" style="37" customWidth="1"/>
-    <col min="3" max="3" width="26.5" style="38" customWidth="1"/>
-    <col min="4" max="4" width="17.125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="28.5" style="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.125" style="38" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.125" style="38" customWidth="1"/>
     <col min="6" max="6" width="30.625" style="38" customWidth="1"/>
     <col min="7" max="16384" width="9" style="8"/>
@@ -3034,39 +3232,39 @@
       <c r="E2" s="42"/>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="189" t="s">
+      <c r="B3" s="190" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="189"/>
-      <c r="D3" s="190" t="str">
+      <c r="C3" s="190"/>
+      <c r="D3" s="191" t="str">
         <f>Cover!C4</f>
         <v>&lt;Project Name&gt;</v>
       </c>
-      <c r="E3" s="190"/>
-      <c r="F3" s="190"/>
+      <c r="E3" s="191"/>
+      <c r="F3" s="191"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="189" t="s">
+      <c r="B4" s="190" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="189"/>
-      <c r="D4" s="190" t="str">
+      <c r="C4" s="190"/>
+      <c r="D4" s="191" t="str">
         <f>Cover!C5</f>
         <v>&lt;Project Code&gt;</v>
       </c>
-      <c r="E4" s="190"/>
-      <c r="F4" s="190"/>
+      <c r="E4" s="191"/>
+      <c r="F4" s="191"/>
     </row>
     <row r="5" spans="2:6" s="43" customFormat="1" ht="84.75" customHeight="1">
-      <c r="B5" s="187" t="s">
+      <c r="B5" s="188" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="187"/>
-      <c r="D5" s="188" t="s">
+      <c r="C5" s="188"/>
+      <c r="D5" s="189" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="188"/>
-      <c r="F5" s="188"/>
+      <c r="E5" s="189"/>
+      <c r="F5" s="189"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="44"/>
@@ -3138,7 +3336,7 @@
       <c r="E11" s="56"/>
       <c r="F11" s="57"/>
     </row>
-    <row r="12" spans="2:6" ht="38.25">
+    <row r="12" spans="2:6" ht="25.5">
       <c r="B12" s="54">
         <v>4</v>
       </c>
@@ -3164,7 +3362,7 @@
       <c r="E13" s="56"/>
       <c r="F13" s="57"/>
     </row>
-    <row r="14" spans="2:6" ht="38.25">
+    <row r="14" spans="2:6" ht="25.5">
       <c r="B14" s="54">
         <v>6</v>
       </c>
@@ -3216,17 +3414,25 @@
       <c r="E17" s="58"/>
       <c r="F17" s="57"/>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" ht="13.5">
       <c r="B18" s="54"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="58"/>
+      <c r="C18" s="55" t="s">
+        <v>244</v>
+      </c>
+      <c r="D18" s="175" t="s">
+        <v>245</v>
+      </c>
       <c r="E18" s="58"/>
       <c r="F18" s="57"/>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" ht="13.5">
       <c r="B19" s="54"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="58"/>
+      <c r="C19" s="55" t="s">
+        <v>246</v>
+      </c>
+      <c r="D19" s="175" t="s">
+        <v>245</v>
+      </c>
       <c r="E19" s="58"/>
       <c r="F19" s="57"/>
     </row>
@@ -3264,6 +3470,8 @@
     <hyperlink ref="D15" location="'Check QLKT-TM screen'!A1" display="Check QLKT-TM screen"/>
     <hyperlink ref="D16" location="'Check QLKT-CN screen'!A1" display="Check QLKT-CN screen"/>
     <hyperlink ref="D17" location="'Check QLKT-CN screen'!A1" display="Check QLKT-CN screen"/>
+    <hyperlink ref="D18" location="'Check QLTL-DS screen'!A1" display="'Check QLTL-DS screen'!A1"/>
+    <hyperlink ref="D19" location="'Check QLTL-DS screen'!A1" display="'Check QLTL-DS screen'!A1"/>
   </hyperlinks>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777783" bottom="1.1506944444444445" header="0.51180555555555562" footer="0.98402777777777783"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3312,13 +3520,13 @@
       <c r="A2" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="192" t="s">
+      <c r="B2" s="193" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="192"/>
-      <c r="D2" s="192"/>
-      <c r="E2" s="192"/>
-      <c r="F2" s="192"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
       <c r="G2" s="72"/>
       <c r="H2" s="43"/>
       <c r="I2" s="69"/>
@@ -3330,13 +3538,13 @@
       <c r="A3" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="192" t="s">
+      <c r="B3" s="193" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="192"/>
-      <c r="D3" s="192"/>
-      <c r="E3" s="192"/>
-      <c r="F3" s="192"/>
+      <c r="C3" s="193"/>
+      <c r="D3" s="193"/>
+      <c r="E3" s="193"/>
+      <c r="F3" s="193"/>
       <c r="G3" s="72"/>
       <c r="H3" s="43"/>
       <c r="I3" s="69"/>
@@ -3348,11 +3556,11 @@
       <c r="A4" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="193"/>
-      <c r="C4" s="193"/>
-      <c r="D4" s="193"/>
-      <c r="E4" s="193"/>
-      <c r="F4" s="193"/>
+      <c r="B4" s="194"/>
+      <c r="C4" s="194"/>
+      <c r="D4" s="194"/>
+      <c r="E4" s="194"/>
+      <c r="F4" s="194"/>
       <c r="G4" s="72"/>
       <c r="H4" s="43"/>
       <c r="I4" s="69"/>
@@ -3371,10 +3579,10 @@
       <c r="D5" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="194" t="s">
+      <c r="E5" s="195" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="194"/>
+      <c r="F5" s="195"/>
       <c r="G5" s="78"/>
       <c r="H5" s="78"/>
       <c r="I5" s="79"/>
@@ -3399,11 +3607,11 @@
         <f>COUNTIF(F$10:F$1002,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="191">
+      <c r="E6" s="192">
         <f>COUNTA(A10:A1002)</f>
         <v>11</v>
       </c>
-      <c r="F6" s="191"/>
+      <c r="F6" s="192"/>
       <c r="G6" s="78"/>
       <c r="H6" s="78"/>
       <c r="I6" s="79"/>
@@ -3772,13 +3980,13 @@
       <c r="A2" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="192" t="s">
+      <c r="B2" s="193" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="192"/>
-      <c r="D2" s="192"/>
-      <c r="E2" s="192"/>
-      <c r="F2" s="192"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
       <c r="G2" s="72"/>
       <c r="H2" s="43"/>
       <c r="I2" s="69"/>
@@ -3790,13 +3998,13 @@
       <c r="A3" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="192" t="s">
+      <c r="B3" s="193" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="192"/>
-      <c r="D3" s="192"/>
-      <c r="E3" s="192"/>
-      <c r="F3" s="192"/>
+      <c r="C3" s="193"/>
+      <c r="D3" s="193"/>
+      <c r="E3" s="193"/>
+      <c r="F3" s="193"/>
       <c r="G3" s="72"/>
       <c r="H3" s="43"/>
       <c r="I3" s="69"/>
@@ -3808,11 +4016,11 @@
       <c r="A4" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="193"/>
-      <c r="C4" s="193"/>
-      <c r="D4" s="193"/>
-      <c r="E4" s="193"/>
-      <c r="F4" s="193"/>
+      <c r="B4" s="194"/>
+      <c r="C4" s="194"/>
+      <c r="D4" s="194"/>
+      <c r="E4" s="194"/>
+      <c r="F4" s="194"/>
       <c r="G4" s="72"/>
       <c r="H4" s="43"/>
       <c r="I4" s="69"/>
@@ -3831,10 +4039,10 @@
       <c r="D5" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="194" t="s">
+      <c r="E5" s="195" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="194"/>
+      <c r="F5" s="195"/>
       <c r="G5" s="78"/>
       <c r="H5" s="78"/>
       <c r="I5" s="79"/>
@@ -3859,11 +4067,11 @@
         <f>COUNTIF(F$10:F$1004,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="191">
+      <c r="E6" s="192">
         <f>COUNTA(A10:A1004)</f>
         <v>6</v>
       </c>
-      <c r="F6" s="191"/>
+      <c r="F6" s="192"/>
       <c r="G6" s="78"/>
       <c r="H6" s="78"/>
       <c r="I6" s="79"/>
@@ -3939,10 +4147,10 @@
       <c r="I10" s="95"/>
     </row>
     <row r="11" spans="1:10" ht="25.5">
-      <c r="A11" s="195" t="s">
+      <c r="A11" s="196" t="s">
         <v>103</v>
       </c>
-      <c r="B11" s="195" t="s">
+      <c r="B11" s="196" t="s">
         <v>104</v>
       </c>
       <c r="C11" s="159"/>
@@ -3958,8 +4166,8 @@
       <c r="I11" s="95"/>
     </row>
     <row r="12" spans="1:10" ht="25.5">
-      <c r="A12" s="196"/>
-      <c r="B12" s="196"/>
+      <c r="A12" s="197"/>
+      <c r="B12" s="197"/>
       <c r="C12" s="159" t="s">
         <v>106</v>
       </c>
@@ -3973,8 +4181,8 @@
       <c r="I12" s="95"/>
     </row>
     <row r="13" spans="1:10" ht="25.5">
-      <c r="A13" s="196"/>
-      <c r="B13" s="196"/>
+      <c r="A13" s="197"/>
+      <c r="B13" s="197"/>
       <c r="C13" s="159" t="s">
         <v>107</v>
       </c>
@@ -3988,8 +4196,8 @@
       <c r="I13" s="95"/>
     </row>
     <row r="14" spans="1:10" ht="25.5">
-      <c r="A14" s="196"/>
-      <c r="B14" s="196"/>
+      <c r="A14" s="197"/>
+      <c r="B14" s="197"/>
       <c r="C14" s="160" t="s">
         <v>108</v>
       </c>
@@ -4003,8 +4211,8 @@
       <c r="I14" s="95"/>
     </row>
     <row r="15" spans="1:10" ht="25.5">
-      <c r="A15" s="196"/>
-      <c r="B15" s="196"/>
+      <c r="A15" s="197"/>
+      <c r="B15" s="197"/>
       <c r="C15" s="160" t="s">
         <v>109</v>
       </c>
@@ -4018,8 +4226,8 @@
       <c r="I15" s="95"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="197"/>
-      <c r="B16" s="197"/>
+      <c r="A16" s="198"/>
+      <c r="B16" s="198"/>
       <c r="C16" s="160" t="s">
         <v>110</v>
       </c>
@@ -4167,7 +4375,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+      <selection activeCell="H5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4200,13 +4408,13 @@
       <c r="A2" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="192" t="s">
+      <c r="B2" s="193" t="s">
         <v>187</v>
       </c>
-      <c r="C2" s="192"/>
-      <c r="D2" s="192"/>
-      <c r="E2" s="192"/>
-      <c r="F2" s="192"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
       <c r="G2" s="72"/>
       <c r="H2" s="43"/>
       <c r="I2" s="69"/>
@@ -4218,13 +4426,13 @@
       <c r="A3" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="192" t="s">
+      <c r="B3" s="193" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="192"/>
-      <c r="D3" s="192"/>
-      <c r="E3" s="192"/>
-      <c r="F3" s="192"/>
+      <c r="C3" s="193"/>
+      <c r="D3" s="193"/>
+      <c r="E3" s="193"/>
+      <c r="F3" s="193"/>
       <c r="G3" s="72"/>
       <c r="H3" s="43"/>
       <c r="I3" s="69"/>
@@ -4236,11 +4444,11 @@
       <c r="A4" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="193"/>
-      <c r="C4" s="193"/>
-      <c r="D4" s="193"/>
-      <c r="E4" s="193"/>
-      <c r="F4" s="193"/>
+      <c r="B4" s="194"/>
+      <c r="C4" s="194"/>
+      <c r="D4" s="194"/>
+      <c r="E4" s="194"/>
+      <c r="F4" s="194"/>
       <c r="G4" s="72"/>
       <c r="H4" s="43"/>
       <c r="I4" s="69"/>
@@ -4259,10 +4467,10 @@
       <c r="D5" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="194" t="s">
+      <c r="E5" s="195" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="194"/>
+      <c r="F5" s="195"/>
       <c r="G5" s="78"/>
       <c r="H5" s="78"/>
       <c r="I5" s="79"/>
@@ -4287,11 +4495,11 @@
         <f>COUNTIF(F$10:F$1008,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="191">
+      <c r="E6" s="192">
         <f>COUNTA(A10:A1009)</f>
         <v>14</v>
       </c>
-      <c r="F6" s="191"/>
+      <c r="F6" s="192"/>
       <c r="G6" s="78"/>
       <c r="H6" s="78"/>
       <c r="I6" s="79"/>
@@ -4734,13 +4942,13 @@
       <c r="A2" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="192" t="s">
+      <c r="B2" s="193" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="192"/>
-      <c r="D2" s="192"/>
-      <c r="E2" s="192"/>
-      <c r="F2" s="192"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
       <c r="G2" s="72"/>
       <c r="H2" s="43"/>
       <c r="I2" s="69"/>
@@ -4752,13 +4960,13 @@
       <c r="A3" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="192" t="s">
+      <c r="B3" s="193" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="192"/>
-      <c r="D3" s="192"/>
-      <c r="E3" s="192"/>
-      <c r="F3" s="192"/>
+      <c r="C3" s="193"/>
+      <c r="D3" s="193"/>
+      <c r="E3" s="193"/>
+      <c r="F3" s="193"/>
       <c r="G3" s="72"/>
       <c r="H3" s="43"/>
       <c r="I3" s="69"/>
@@ -4770,11 +4978,11 @@
       <c r="A4" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="193"/>
-      <c r="C4" s="193"/>
-      <c r="D4" s="193"/>
-      <c r="E4" s="193"/>
-      <c r="F4" s="193"/>
+      <c r="B4" s="194"/>
+      <c r="C4" s="194"/>
+      <c r="D4" s="194"/>
+      <c r="E4" s="194"/>
+      <c r="F4" s="194"/>
       <c r="G4" s="72"/>
       <c r="H4" s="43"/>
       <c r="I4" s="69"/>
@@ -4793,10 +5001,10 @@
       <c r="D5" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="194" t="s">
+      <c r="E5" s="195" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="194"/>
+      <c r="F5" s="195"/>
       <c r="G5" s="78"/>
       <c r="H5" s="78"/>
       <c r="I5" s="79"/>
@@ -4821,11 +5029,11 @@
         <f>COUNTIF(F$10:F$1011,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="191">
+      <c r="E6" s="192">
         <f>COUNTA(A10:A1012)</f>
         <v>17</v>
       </c>
-      <c r="F6" s="191"/>
+      <c r="F6" s="192"/>
       <c r="G6" s="78"/>
       <c r="H6" s="78"/>
       <c r="I6" s="79"/>
@@ -5284,32 +5492,32 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9" style="8"/>
     <col min="2" max="2" width="13.5" style="8" customWidth="1"/>
-    <col min="3" max="3" width="19.375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="30.875" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="9" style="8"/>
     <col min="8" max="9" width="33.125" style="8" customWidth="1"/>
     <col min="10" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.5" customHeight="1">
-      <c r="B1" s="200" t="s">
+      <c r="B1" s="201" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
-      <c r="E1" s="200"/>
-      <c r="F1" s="200"/>
-      <c r="G1" s="200"/>
-      <c r="H1" s="200"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+      <c r="E1" s="201"/>
+      <c r="F1" s="201"/>
+      <c r="G1" s="201"/>
+      <c r="H1" s="201"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1">
       <c r="A2" s="105"/>
@@ -5325,14 +5533,14 @@
       <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="190" t="s">
+      <c r="C3" s="191" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="190"/>
-      <c r="E3" s="198" t="s">
+      <c r="D3" s="191"/>
+      <c r="E3" s="199" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="198"/>
+      <c r="F3" s="199"/>
       <c r="G3" s="108"/>
       <c r="H3" s="109"/>
     </row>
@@ -5340,14 +5548,14 @@
       <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="190" t="s">
+      <c r="C4" s="191" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="190"/>
-      <c r="E4" s="198" t="s">
+      <c r="D4" s="191"/>
+      <c r="E4" s="199" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="198"/>
+      <c r="F4" s="199"/>
       <c r="G4" s="108"/>
       <c r="H4" s="109"/>
     </row>
@@ -5355,15 +5563,15 @@
       <c r="B5" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="190" t="str">
+      <c r="C5" s="191" t="str">
         <f>C4&amp;"_"&amp;"Test Report"&amp;"_"&amp;"vx.x"</f>
         <v>&lt;Project Code&gt;_Test Report_vx.x</v>
       </c>
-      <c r="D5" s="190"/>
-      <c r="E5" s="198" t="s">
+      <c r="D5" s="191"/>
+      <c r="E5" s="199" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="198"/>
+      <c r="F5" s="199"/>
       <c r="G5" s="108"/>
       <c r="H5" s="111" t="s">
         <v>44</v>
@@ -5374,14 +5582,14 @@
       <c r="B6" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="199" t="s">
+      <c r="C6" s="200" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="199"/>
-      <c r="E6" s="199"/>
-      <c r="F6" s="199"/>
-      <c r="G6" s="199"/>
-      <c r="H6" s="199"/>
+      <c r="D6" s="200"/>
+      <c r="E6" s="200"/>
+      <c r="F6" s="200"/>
+      <c r="G6" s="200"/>
+      <c r="H6" s="200"/>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1">
       <c r="A7" s="105"/>
@@ -5532,80 +5740,112 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="25.5">
       <c r="A15" s="121"/>
-      <c r="B15" s="127"/>
-      <c r="C15" s="128" t="s">
+      <c r="B15" s="178"/>
+      <c r="C15" s="179" t="s">
+        <v>247</v>
+      </c>
+      <c r="D15" s="180">
+        <v>6</v>
+      </c>
+      <c r="E15" s="180"/>
+      <c r="F15" s="180"/>
+      <c r="G15" s="181"/>
+      <c r="H15" s="182">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="121"/>
+      <c r="B16" s="178"/>
+      <c r="C16" s="179" t="s">
+        <v>279</v>
+      </c>
+      <c r="D16" s="180">
+        <v>16</v>
+      </c>
+      <c r="E16" s="180"/>
+      <c r="F16" s="180"/>
+      <c r="G16" s="181"/>
+      <c r="H16" s="182">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="121"/>
+      <c r="B17" s="127"/>
+      <c r="C17" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="129">
-        <f>SUM(D9:D14)</f>
-        <v>48</v>
-      </c>
-      <c r="E15" s="129">
+      <c r="D17" s="129">
+        <f>SUM(D9:D16)</f>
+        <v>70</v>
+      </c>
+      <c r="E17" s="129">
         <f>SUM(E9:E13)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="129">
+      <c r="F17" s="129">
         <f>SUM(F9:F13)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="129">
+      <c r="G17" s="129">
         <f>SUM(G9:G13)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="130">
-        <f>SUM(H9:H14)</f>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="114"/>
-      <c r="B16" s="131"/>
-      <c r="C16" s="114"/>
-      <c r="D16" s="132"/>
-      <c r="E16" s="133"/>
-      <c r="F16" s="133"/>
-      <c r="G16" s="133"/>
-      <c r="H16" s="133"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="114"/>
-      <c r="B17" s="114"/>
-      <c r="C17" s="134" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="114"/>
-      <c r="E17" s="135">
-        <f>(D15+E15)*100/(H15-G15)</f>
-        <v>100</v>
-      </c>
-      <c r="F17" s="114" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" s="114"/>
-      <c r="H17" s="83"/>
+      <c r="H17" s="130">
+        <f>SUM(H9:H16)</f>
+        <v>70</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="114"/>
-      <c r="B18" s="114"/>
-      <c r="C18" s="134" t="s">
+      <c r="B18" s="131"/>
+      <c r="C18" s="114"/>
+      <c r="D18" s="132"/>
+      <c r="E18" s="133"/>
+      <c r="F18" s="133"/>
+      <c r="G18" s="133"/>
+      <c r="H18" s="133"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="114"/>
+      <c r="B19" s="114"/>
+      <c r="C19" s="134" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="114"/>
+      <c r="E19" s="135">
+        <f>(D17+E17)*100/(H17-G17)</f>
+        <v>100</v>
+      </c>
+      <c r="F19" s="114" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="114"/>
+      <c r="H19" s="83"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="114"/>
+      <c r="B20" s="114"/>
+      <c r="C20" s="134" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="114"/>
-      <c r="E18" s="135">
-        <f>D15*100/(H15-G15)</f>
+      <c r="D20" s="114"/>
+      <c r="E20" s="135">
+        <f>D17*100/(H17-G17)</f>
         <v>100</v>
       </c>
-      <c r="F18" s="114" t="s">
+      <c r="F20" s="114" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="114"/>
-      <c r="H18" s="83"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="C19" s="114"/>
-      <c r="D19" s="114"/>
+      <c r="G20" s="114"/>
+      <c r="H20" s="83"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="C21" s="114"/>
+      <c r="D21" s="114"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5631,8 +5871,426 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="11.5" style="8" customWidth="1"/>
+    <col min="2" max="2" width="19.125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="25.625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="30.125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="16.875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="7.125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="9" style="63"/>
+    <col min="8" max="8" width="17.625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="8.25" style="64" customWidth="1"/>
+    <col min="10" max="10" width="0" style="8" hidden="1" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="70" customFormat="1" ht="13.5" thickBot="1">
+      <c r="A1" s="65"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="69"/>
+    </row>
+    <row r="2" spans="1:10" s="70" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="71" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="193" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="70" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="70" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A3" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="193" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="193"/>
+      <c r="D3" s="193"/>
+      <c r="E3" s="193"/>
+      <c r="F3" s="193"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="70" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="70" customFormat="1" ht="18" customHeight="1">
+      <c r="A4" s="71" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="194"/>
+      <c r="C4" s="194"/>
+      <c r="D4" s="194"/>
+      <c r="E4" s="194"/>
+      <c r="F4" s="194"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="74"/>
+    </row>
+    <row r="5" spans="1:10" s="70" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A5" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="76" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="77" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="195" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="195"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="70" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="70" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A6" s="101">
+        <v>6</v>
+      </c>
+      <c r="B6" s="81">
+        <f>COUNTIF(F10:F1004,"Fail")</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="81">
+        <f>E6-D6-B6-A6</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="82">
+        <f>COUNTIF(F$10:F$1004,"N/A")</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="192">
+        <v>6</v>
+      </c>
+      <c r="F6" s="192"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="70" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="70" customFormat="1" ht="15" customHeight="1">
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="79"/>
+    </row>
+    <row r="8" spans="1:10" s="70" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A8" s="84" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="84" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="84" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="84" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="85" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="85" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="85" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="84" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="86"/>
+    </row>
+    <row r="9" spans="1:10" s="70" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A9" s="87"/>
+      <c r="B9" s="87" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="89"/>
+      <c r="I9" s="90"/>
+    </row>
+    <row r="10" spans="1:10" s="96" customFormat="1" ht="120.95" customHeight="1">
+      <c r="A10" s="141" t="s">
+        <v>231</v>
+      </c>
+      <c r="B10" s="157" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="153"/>
+      <c r="D10" s="151" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="154"/>
+      <c r="F10" s="91" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="91"/>
+      <c r="H10" s="102"/>
+      <c r="I10" s="95"/>
+    </row>
+    <row r="11" spans="1:10" ht="25.5">
+      <c r="A11" s="196" t="s">
+        <v>240</v>
+      </c>
+      <c r="B11" s="196" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="159"/>
+      <c r="D11" s="147" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="148"/>
+      <c r="F11" s="152" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="91"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="95"/>
+    </row>
+    <row r="12" spans="1:10" ht="25.5">
+      <c r="A12" s="197"/>
+      <c r="B12" s="197"/>
+      <c r="C12" s="159" t="s">
+        <v>232</v>
+      </c>
+      <c r="D12" s="147" t="s">
+        <v>236</v>
+      </c>
+      <c r="E12" s="148"/>
+      <c r="F12" s="152"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="102"/>
+      <c r="I12" s="95"/>
+    </row>
+    <row r="13" spans="1:10" ht="25.5">
+      <c r="A13" s="197"/>
+      <c r="B13" s="197"/>
+      <c r="C13" s="159" t="s">
+        <v>233</v>
+      </c>
+      <c r="D13" s="147" t="s">
+        <v>237</v>
+      </c>
+      <c r="E13" s="148"/>
+      <c r="F13" s="152"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="102"/>
+      <c r="I13" s="95"/>
+    </row>
+    <row r="14" spans="1:10" ht="25.5">
+      <c r="A14" s="197"/>
+      <c r="B14" s="197"/>
+      <c r="C14" s="160" t="s">
+        <v>234</v>
+      </c>
+      <c r="D14" s="155" t="s">
+        <v>238</v>
+      </c>
+      <c r="E14" s="158"/>
+      <c r="F14" s="152"/>
+      <c r="G14" s="91"/>
+      <c r="H14" s="102"/>
+      <c r="I14" s="95"/>
+    </row>
+    <row r="15" spans="1:10" ht="25.5">
+      <c r="A15" s="197"/>
+      <c r="B15" s="197"/>
+      <c r="C15" s="160" t="s">
+        <v>235</v>
+      </c>
+      <c r="D15" s="155" t="s">
+        <v>239</v>
+      </c>
+      <c r="E15" s="158"/>
+      <c r="F15" s="152"/>
+      <c r="G15" s="91"/>
+      <c r="H15" s="102"/>
+      <c r="I15" s="95"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="198"/>
+      <c r="B16" s="198"/>
+      <c r="C16" s="160" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="155" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="158"/>
+      <c r="F16" s="152"/>
+      <c r="G16" s="91"/>
+      <c r="H16" s="102"/>
+      <c r="I16" s="95"/>
+    </row>
+    <row r="17" spans="1:11" ht="25.5">
+      <c r="A17" s="162" t="s">
+        <v>241</v>
+      </c>
+      <c r="B17" s="163" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="164"/>
+      <c r="D17" s="156" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="165"/>
+      <c r="F17" s="166" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="141"/>
+      <c r="H17" s="167"/>
+      <c r="I17" s="95"/>
+    </row>
+    <row r="18" spans="1:11" ht="25.5">
+      <c r="A18" s="142" t="s">
+        <v>242</v>
+      </c>
+      <c r="B18" s="142" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="142"/>
+      <c r="D18" s="147" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="148"/>
+      <c r="F18" s="142" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="142"/>
+      <c r="H18" s="169"/>
+      <c r="I18" s="95"/>
+    </row>
+    <row r="19" spans="1:11" s="70" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A19" s="146"/>
+      <c r="B19" s="146" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" s="140"/>
+      <c r="D19" s="140"/>
+      <c r="E19" s="140"/>
+      <c r="F19" s="140"/>
+      <c r="G19" s="140"/>
+      <c r="H19" s="168"/>
+      <c r="I19" s="90"/>
+    </row>
+    <row r="20" spans="1:11" ht="51">
+      <c r="A20" s="91" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="91" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" s="149" t="s">
+        <v>243</v>
+      </c>
+      <c r="D20" s="149" t="s">
+        <v>124</v>
+      </c>
+      <c r="E20" s="91"/>
+      <c r="F20" s="91" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="91"/>
+      <c r="H20" s="102"/>
+      <c r="I20" s="95"/>
+    </row>
+    <row r="21" spans="1:11" ht="51">
+      <c r="A21" s="91" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="91" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="149" t="s">
+        <v>243</v>
+      </c>
+      <c r="D21" s="149" t="s">
+        <v>128</v>
+      </c>
+      <c r="E21" s="91"/>
+      <c r="F21" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="98"/>
+      <c r="H21" s="99"/>
+      <c r="I21" s="100"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="F22" s="103"/>
+      <c r="I22" s="90"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="70"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="F23" s="104"/>
+      <c r="I23" s="95"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F3 F7:F150">
+      <formula1>$J$2:$J$6</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5665,13 +6323,13 @@
       <c r="A2" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="192" t="s">
-        <v>230</v>
-      </c>
-      <c r="C2" s="192"/>
-      <c r="D2" s="192"/>
-      <c r="E2" s="192"/>
-      <c r="F2" s="192"/>
+      <c r="B2" s="193" t="s">
+        <v>248</v>
+      </c>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
       <c r="G2" s="72"/>
       <c r="H2" s="43"/>
       <c r="I2" s="69"/>
@@ -5683,13 +6341,13 @@
       <c r="A3" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="192" t="s">
+      <c r="B3" s="193" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="192"/>
-      <c r="D3" s="192"/>
-      <c r="E3" s="192"/>
-      <c r="F3" s="192"/>
+      <c r="C3" s="193"/>
+      <c r="D3" s="193"/>
+      <c r="E3" s="193"/>
+      <c r="F3" s="193"/>
       <c r="G3" s="72"/>
       <c r="H3" s="43"/>
       <c r="I3" s="69"/>
@@ -5701,11 +6359,11 @@
       <c r="A4" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="193"/>
-      <c r="C4" s="193"/>
-      <c r="D4" s="193"/>
-      <c r="E4" s="193"/>
-      <c r="F4" s="193"/>
+      <c r="B4" s="194"/>
+      <c r="C4" s="194"/>
+      <c r="D4" s="194"/>
+      <c r="E4" s="194"/>
+      <c r="F4" s="194"/>
       <c r="G4" s="72"/>
       <c r="H4" s="43"/>
       <c r="I4" s="69"/>
@@ -5724,10 +6382,10 @@
       <c r="D5" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="194" t="s">
+      <c r="E5" s="195" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="194"/>
+      <c r="F5" s="195"/>
       <c r="G5" s="78"/>
       <c r="H5" s="78"/>
       <c r="I5" s="79"/>
@@ -5737,10 +6395,10 @@
     </row>
     <row r="6" spans="1:10" s="70" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="101">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B6" s="81">
-        <f>COUNTIF(F10:F1004,"Fail")</f>
+        <f>COUNTIF(F10:F1010,"Fail")</f>
         <v>0</v>
       </c>
       <c r="C6" s="81">
@@ -5748,13 +6406,13 @@
         <v>0</v>
       </c>
       <c r="D6" s="82">
-        <f>COUNTIF(F$10:F$1004,"N/A")</f>
+        <f>COUNTIF(F$10:F$1010,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="191">
-        <v>2</v>
-      </c>
-      <c r="F6" s="191"/>
+      <c r="E6" s="192">
+        <v>16</v>
+      </c>
+      <c r="F6" s="192"/>
       <c r="G6" s="78"/>
       <c r="H6" s="78"/>
       <c r="I6" s="79"/>
@@ -5800,7 +6458,7 @@
     <row r="9" spans="1:10" s="70" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="87"/>
       <c r="B9" s="87" t="s">
-        <v>120</v>
+        <v>257</v>
       </c>
       <c r="C9" s="88"/>
       <c r="D9" s="88"/>
@@ -5811,34 +6469,34 @@
       <c r="I9" s="90"/>
     </row>
     <row r="10" spans="1:10" s="96" customFormat="1" ht="120.95" customHeight="1">
-      <c r="A10" s="141" t="s">
-        <v>231</v>
-      </c>
-      <c r="B10" s="157" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="153"/>
-      <c r="D10" s="151" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="154"/>
-      <c r="F10" s="91" t="s">
+      <c r="A10" s="183" t="s">
+        <v>249</v>
+      </c>
+      <c r="B10" s="171" t="s">
+        <v>250</v>
+      </c>
+      <c r="C10" s="159"/>
+      <c r="D10" s="147" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="148"/>
+      <c r="F10" s="152" t="s">
         <v>26</v>
       </c>
       <c r="G10" s="91"/>
       <c r="H10" s="102"/>
       <c r="I10" s="95"/>
     </row>
-    <row r="11" spans="1:10" ht="25.5">
-      <c r="A11" s="195" t="s">
-        <v>240</v>
-      </c>
-      <c r="B11" s="195" t="s">
-        <v>104</v>
+    <row r="11" spans="1:10" ht="63.75" customHeight="1">
+      <c r="A11" s="170" t="s">
+        <v>251</v>
+      </c>
+      <c r="B11" s="172" t="s">
+        <v>255</v>
       </c>
       <c r="C11" s="159"/>
       <c r="D11" s="147" t="s">
-        <v>105</v>
+        <v>59</v>
       </c>
       <c r="E11" s="148"/>
       <c r="F11" s="152" t="s">
@@ -5848,165 +6506,193 @@
       <c r="H11" s="102"/>
       <c r="I11" s="95"/>
     </row>
-    <row r="12" spans="1:10" ht="25.5">
-      <c r="A12" s="196"/>
-      <c r="B12" s="196"/>
-      <c r="C12" s="159" t="s">
-        <v>232</v>
-      </c>
+    <row r="12" spans="1:10" ht="51" customHeight="1">
+      <c r="A12" s="170" t="s">
+        <v>252</v>
+      </c>
+      <c r="B12" s="172" t="s">
+        <v>256</v>
+      </c>
+      <c r="C12" s="159"/>
       <c r="D12" s="147" t="s">
-        <v>236</v>
+        <v>59</v>
       </c>
       <c r="E12" s="148"/>
-      <c r="F12" s="152"/>
+      <c r="F12" s="152" t="s">
+        <v>26</v>
+      </c>
       <c r="G12" s="91"/>
       <c r="H12" s="102"/>
       <c r="I12" s="95"/>
     </row>
-    <row r="13" spans="1:10" ht="25.5">
-      <c r="A13" s="196"/>
-      <c r="B13" s="196"/>
-      <c r="C13" s="159" t="s">
-        <v>233</v>
-      </c>
-      <c r="D13" s="147" t="s">
-        <v>237</v>
-      </c>
-      <c r="E13" s="148"/>
-      <c r="F13" s="152"/>
+    <row r="13" spans="1:10" ht="51" customHeight="1">
+      <c r="A13" s="170" t="s">
+        <v>253</v>
+      </c>
+      <c r="B13" s="172" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" s="160"/>
+      <c r="D13" s="155" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="158"/>
+      <c r="F13" s="152" t="s">
+        <v>26</v>
+      </c>
       <c r="G13" s="91"/>
       <c r="H13" s="102"/>
       <c r="I13" s="95"/>
     </row>
-    <row r="14" spans="1:10" ht="25.5">
-      <c r="A14" s="196"/>
-      <c r="B14" s="196"/>
-      <c r="C14" s="160" t="s">
-        <v>234</v>
-      </c>
+    <row r="14" spans="1:10" ht="51" customHeight="1">
+      <c r="A14" s="170" t="s">
+        <v>254</v>
+      </c>
+      <c r="B14" s="172" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" s="160"/>
       <c r="D14" s="155" t="s">
-        <v>238</v>
+        <v>64</v>
       </c>
       <c r="E14" s="158"/>
-      <c r="F14" s="152"/>
+      <c r="F14" s="152" t="s">
+        <v>26</v>
+      </c>
       <c r="G14" s="91"/>
       <c r="H14" s="102"/>
       <c r="I14" s="95"/>
     </row>
-    <row r="15" spans="1:10" ht="25.5">
-      <c r="A15" s="196"/>
-      <c r="B15" s="196"/>
-      <c r="C15" s="160" t="s">
-        <v>235</v>
-      </c>
-      <c r="D15" s="155" t="s">
-        <v>239</v>
-      </c>
-      <c r="E15" s="158"/>
-      <c r="F15" s="152"/>
-      <c r="G15" s="91"/>
-      <c r="H15" s="102"/>
+    <row r="15" spans="1:10" ht="63.75" customHeight="1">
+      <c r="A15" s="146"/>
+      <c r="B15" s="146" t="s">
+        <v>202</v>
+      </c>
+      <c r="C15" s="140"/>
+      <c r="D15" s="140"/>
+      <c r="E15" s="140"/>
+      <c r="F15" s="140"/>
+      <c r="G15" s="140"/>
+      <c r="H15" s="168"/>
       <c r="I15" s="95"/>
     </row>
-    <row r="16" spans="1:10" ht="25.5">
-      <c r="A16" s="197"/>
-      <c r="B16" s="197"/>
-      <c r="C16" s="160" t="s">
-        <v>110</v>
-      </c>
-      <c r="D16" s="155" t="s">
-        <v>115</v>
-      </c>
-      <c r="E16" s="158"/>
-      <c r="F16" s="152"/>
+    <row r="16" spans="1:10" s="70" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A16" s="91" t="s">
+        <v>192</v>
+      </c>
+      <c r="B16" s="91" t="s">
+        <v>203</v>
+      </c>
+      <c r="C16" s="149" t="s">
+        <v>258</v>
+      </c>
+      <c r="D16" s="149" t="s">
+        <v>205</v>
+      </c>
+      <c r="E16" s="91"/>
+      <c r="F16" s="91" t="s">
+        <v>26</v>
+      </c>
       <c r="G16" s="91"/>
       <c r="H16" s="102"/>
-      <c r="I16" s="95"/>
-    </row>
-    <row r="17" spans="1:11" ht="25.5">
-      <c r="A17" s="162" t="s">
-        <v>241</v>
-      </c>
-      <c r="B17" s="163" t="s">
-        <v>117</v>
-      </c>
-      <c r="C17" s="164"/>
-      <c r="D17" s="156" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="165"/>
-      <c r="F17" s="166" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" s="141"/>
-      <c r="H17" s="167"/>
+      <c r="I16" s="90"/>
+    </row>
+    <row r="17" spans="1:11" ht="63.75">
+      <c r="A17" s="91" t="s">
+        <v>193</v>
+      </c>
+      <c r="B17" s="91" t="s">
+        <v>206</v>
+      </c>
+      <c r="C17" s="149" t="s">
+        <v>259</v>
+      </c>
+      <c r="D17" s="149" t="s">
+        <v>260</v>
+      </c>
+      <c r="E17" s="91"/>
+      <c r="F17" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="98"/>
+      <c r="H17" s="99"/>
       <c r="I17" s="95"/>
     </row>
-    <row r="18" spans="1:11" ht="25.5">
-      <c r="A18" s="142" t="s">
-        <v>242</v>
-      </c>
-      <c r="B18" s="142" t="s">
-        <v>119</v>
-      </c>
-      <c r="C18" s="142"/>
-      <c r="D18" s="147" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" s="148"/>
-      <c r="F18" s="142" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="142"/>
-      <c r="H18" s="169"/>
+    <row r="18" spans="1:11" ht="63.75">
+      <c r="A18" s="91" t="s">
+        <v>194</v>
+      </c>
+      <c r="B18" s="91" t="s">
+        <v>261</v>
+      </c>
+      <c r="C18" s="149" t="s">
+        <v>264</v>
+      </c>
+      <c r="D18" s="149" t="s">
+        <v>262</v>
+      </c>
+      <c r="E18" s="91"/>
+      <c r="F18" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" s="98"/>
+      <c r="H18" s="99"/>
       <c r="I18" s="95"/>
     </row>
-    <row r="19" spans="1:11" s="70" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A19" s="146"/>
-      <c r="B19" s="146" t="s">
-        <v>121</v>
-      </c>
-      <c r="C19" s="140"/>
-      <c r="D19" s="140"/>
-      <c r="E19" s="140"/>
-      <c r="F19" s="140"/>
-      <c r="G19" s="140"/>
-      <c r="H19" s="168"/>
-      <c r="I19" s="90"/>
-    </row>
-    <row r="20" spans="1:11" ht="178.5">
+    <row r="19" spans="1:11" ht="76.5">
+      <c r="A19" s="91" t="s">
+        <v>195</v>
+      </c>
+      <c r="B19" s="91" t="s">
+        <v>263</v>
+      </c>
+      <c r="C19" s="149" t="s">
+        <v>265</v>
+      </c>
+      <c r="D19" s="149" t="s">
+        <v>268</v>
+      </c>
+      <c r="E19" s="91"/>
+      <c r="F19" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="98"/>
+      <c r="H19" s="99"/>
+      <c r="I19" s="95"/>
+    </row>
+    <row r="20" spans="1:11" ht="76.5">
       <c r="A20" s="91" t="s">
-        <v>122</v>
+        <v>196</v>
       </c>
       <c r="B20" s="91" t="s">
-        <v>123</v>
+        <v>266</v>
       </c>
       <c r="C20" s="149" t="s">
-        <v>127</v>
+        <v>267</v>
       </c>
       <c r="D20" s="149" t="s">
-        <v>124</v>
+        <v>269</v>
       </c>
       <c r="E20" s="91"/>
-      <c r="F20" s="91" t="s">
-        <v>26</v>
-      </c>
-      <c r="G20" s="91"/>
-      <c r="H20" s="102"/>
+      <c r="F20" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="98"/>
+      <c r="H20" s="99"/>
       <c r="I20" s="95"/>
     </row>
-    <row r="21" spans="1:11" ht="153">
+    <row r="21" spans="1:11" ht="63.75">
       <c r="A21" s="91" t="s">
-        <v>125</v>
+        <v>197</v>
       </c>
       <c r="B21" s="91" t="s">
-        <v>126</v>
+        <v>271</v>
       </c>
       <c r="C21" s="149" t="s">
-        <v>127</v>
+        <v>270</v>
       </c>
       <c r="D21" s="149" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="E21" s="91"/>
       <c r="F21" s="99" t="s">
@@ -6014,30 +6700,156 @@
       </c>
       <c r="G21" s="98"/>
       <c r="H21" s="99"/>
-      <c r="I21" s="100"/>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="F22" s="103"/>
-      <c r="I22" s="90"/>
-      <c r="J22" s="70"/>
-      <c r="K22" s="70"/>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="F23" s="104"/>
+      <c r="I21" s="95"/>
+    </row>
+    <row r="22" spans="1:11" ht="63.75">
+      <c r="A22" s="91" t="s">
+        <v>198</v>
+      </c>
+      <c r="B22" s="91" t="s">
+        <v>272</v>
+      </c>
+      <c r="C22" s="149" t="s">
+        <v>280</v>
+      </c>
+      <c r="D22" s="149" t="s">
+        <v>273</v>
+      </c>
+      <c r="E22" s="91"/>
+      <c r="F22" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="98"/>
+      <c r="H22" s="99"/>
+      <c r="I22" s="95"/>
+    </row>
+    <row r="23" spans="1:11" ht="63.75">
+      <c r="A23" s="91" t="s">
+        <v>199</v>
+      </c>
+      <c r="B23" s="91" t="s">
+        <v>281</v>
+      </c>
+      <c r="C23" s="149" t="s">
+        <v>282</v>
+      </c>
+      <c r="D23" s="149" t="s">
+        <v>283</v>
+      </c>
+      <c r="E23" s="91"/>
+      <c r="F23" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="98"/>
+      <c r="H23" s="99"/>
       <c r="I23" s="95"/>
     </row>
+    <row r="24" spans="1:11" ht="63.75">
+      <c r="A24" s="91" t="s">
+        <v>200</v>
+      </c>
+      <c r="B24" s="91" t="s">
+        <v>284</v>
+      </c>
+      <c r="C24" s="149" t="s">
+        <v>285</v>
+      </c>
+      <c r="D24" s="149" t="s">
+        <v>286</v>
+      </c>
+      <c r="E24" s="91"/>
+      <c r="F24" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="98"/>
+      <c r="H24" s="99"/>
+      <c r="I24" s="95"/>
+    </row>
+    <row r="25" spans="1:11" ht="76.5">
+      <c r="A25" s="91" t="s">
+        <v>288</v>
+      </c>
+      <c r="B25" s="91" t="s">
+        <v>274</v>
+      </c>
+      <c r="C25" s="149" t="s">
+        <v>275</v>
+      </c>
+      <c r="D25" s="149" t="s">
+        <v>276</v>
+      </c>
+      <c r="E25" s="91"/>
+      <c r="F25" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="98"/>
+      <c r="H25" s="99"/>
+      <c r="I25" s="95"/>
+    </row>
+    <row r="26" spans="1:11" ht="38.25">
+      <c r="A26" s="91" t="s">
+        <v>287</v>
+      </c>
+      <c r="B26" s="91" t="s">
+        <v>221</v>
+      </c>
+      <c r="C26" s="149" t="s">
+        <v>277</v>
+      </c>
+      <c r="D26" s="149" t="s">
+        <v>278</v>
+      </c>
+      <c r="E26" s="91"/>
+      <c r="F26" s="91" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="91"/>
+      <c r="H26" s="102"/>
+      <c r="I26" s="95"/>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="G27" s="8"/>
+      <c r="I27" s="95"/>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="104"/>
+      <c r="B28" s="104"/>
+      <c r="C28" s="173"/>
+      <c r="D28" s="173"/>
+      <c r="E28" s="104"/>
+      <c r="F28" s="174"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="114"/>
+      <c r="I28" s="95"/>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="F29" s="104"/>
+      <c r="I29" s="95"/>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="I30" s="95"/>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="I31" s="95"/>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="I32" s="90"/>
+      <c r="J32" s="70"/>
+      <c r="K32" s="70"/>
+    </row>
+    <row r="33" spans="9:9">
+      <c r="I33" s="95"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="5">
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A11:A16"/>
-    <mergeCell ref="B11:B16"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F3 F7:F150">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F3 F28:F156 F7:F26">
       <formula1>$J$2:$J$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6045,16 +6857,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>